<commit_message>
a-soft bufixes, improvements & tests for backend
</commit_message>
<xml_diff>
--- a/api/src/test/resources/Trial3_questions_CP_OST_20190911_2_errorTest.xlsx
+++ b/api/src/test/resources/Trial3_questions_CP_OST_20190911_2_errorTest.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projekty git\itti_driver\api\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F46E6CEB-B5C5-4C88-AF34-37E660C25814}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7EDFD57-D330-456E-BC3B-F09F59A921D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="810" yWindow="-120" windowWidth="24510" windowHeight="15990" tabRatio="501" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25335" yWindow="3465" windowWidth="18795" windowHeight="11505" tabRatio="501" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Observer" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5358" uniqueCount="291">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5354" uniqueCount="291">
   <si>
     <t>TrialName</t>
   </si>
@@ -1904,9 +1904,9 @@
   </sheetPr>
   <dimension ref="A1:U407"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P8" sqref="P8"/>
+      <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2063,7 +2063,7 @@
       <c r="D3" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="21" t="s">
         <v>52</v>
       </c>
       <c r="F3" s="8"/>
@@ -2082,18 +2082,10 @@
       <c r="K3" s="8">
         <v>1</v>
       </c>
-      <c r="L3" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="M3" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="N3" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="O3" s="8" t="s">
-        <v>25</v>
-      </c>
+      <c r="L3" s="8"/>
+      <c r="M3" s="8"/>
+      <c r="N3" s="8"/>
+      <c r="O3" s="8"/>
       <c r="P3" s="8"/>
       <c r="Q3" s="8"/>
       <c r="R3" s="8"/>
@@ -25210,7 +25202,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H239 H237 H241 H243 H245">
+  <conditionalFormatting sqref="H237 H239 H241 H243 H245">
     <cfRule type="colorScale" priority="855">
       <colorScale>
         <cfvo type="min"/>
@@ -25250,7 +25242,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O13 L13 J13:J14 F13:F14">
+  <conditionalFormatting sqref="L13 O13 J13:J14 F13:F14">
     <cfRule type="colorScale" priority="818">
       <colorScale>
         <cfvo type="min"/>
@@ -25420,7 +25412,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J100 F100 R100:BO100">
+  <conditionalFormatting sqref="F100 J100 R100:BO100">
     <cfRule type="colorScale" priority="706">
       <colorScale>
         <cfvo type="min"/>
@@ -25450,7 +25442,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M74 O74 S71:S87 U71:U87 W71:W87 F71:F73 F74:G87 O80:O83">
+  <conditionalFormatting sqref="O74 M74 S71:S87 U71:U87 W71:W87 F71:F73 F74:G87 O80:O83">
     <cfRule type="colorScale" priority="702">
       <colorScale>
         <cfvo type="min"/>
@@ -25730,7 +25722,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J128 F128">
+  <conditionalFormatting sqref="F128 J128">
     <cfRule type="colorScale" priority="647">
       <colorScale>
         <cfvo type="min"/>
@@ -25900,7 +25892,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F245 P242 O245 J245">
+  <conditionalFormatting sqref="P242 F245 O245 J245">
     <cfRule type="colorScale" priority="608">
       <colorScale>
         <cfvo type="min"/>
@@ -26650,7 +26642,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F334 J334 L334 N334:O334">
+  <conditionalFormatting sqref="J334 F334 L334 N334:O334">
     <cfRule type="colorScale" priority="444">
       <colorScale>
         <cfvo type="min"/>
@@ -26900,7 +26892,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F200 J200">
+  <conditionalFormatting sqref="J200 F200">
     <cfRule type="colorScale" priority="404">
       <colorScale>
         <cfvo type="min"/>
@@ -26990,7 +26982,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F170 J170">
+  <conditionalFormatting sqref="J170 F170">
     <cfRule type="colorScale" priority="380">
       <colorScale>
         <cfvo type="min"/>
@@ -27620,7 +27612,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J47 J45">
+  <conditionalFormatting sqref="J45 J47">
     <cfRule type="colorScale" priority="283">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>